<commit_message>
Added minimum viable documentation.
</commit_message>
<xml_diff>
--- a/tests/validation-BnB_3p228mm/BnB_3p228mm-Results.xlsx
+++ b/tests/validation-BnB_3p228mm/BnB_3p228mm-Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcellob\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation-BnB_3p228mm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation-BnB_3p228mm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99FE392-EA7E-46D4-B8AE-BDB239807FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16F8790-7801-4A06-94B6-516BCECA86E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -4687,6 +4687,35 @@
     <xf numFmtId="166" fontId="6" fillId="8" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4705,35 +4734,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="8" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5642,7 +5642,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5680,7 +5680,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -5764,7 +5764,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5802,7 +5802,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -5845,7 +5845,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6599,7 +6599,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6637,7 +6637,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -6722,7 +6722,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6760,7 +6760,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -6803,7 +6803,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7557,7 +7557,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7595,7 +7595,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -7679,7 +7679,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7717,7 +7717,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -7760,7 +7760,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8514,7 +8514,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8552,7 +8552,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -8637,7 +8637,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8675,7 +8675,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -8718,7 +8718,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9472,7 +9472,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9510,7 +9510,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -9594,7 +9594,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9632,7 +9632,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -9675,7 +9675,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10429,7 +10429,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10467,7 +10467,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -10552,7 +10552,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10590,7 +10590,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -10633,7 +10633,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11387,7 +11387,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11425,7 +11425,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -11509,7 +11509,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11547,7 +11547,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -11590,7 +11590,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12344,7 +12344,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12382,7 +12382,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -12467,7 +12467,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12505,7 +12505,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -12548,7 +12548,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -18056,32 +18056,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -18097,12 +18097,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="155"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="166"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -18110,12 +18110,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="155"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="166"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -18123,12 +18123,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="155"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="166"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -18136,12 +18136,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="155"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="166"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -18149,12 +18149,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="155"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -18202,112 +18202,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="167" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="158" t="s">
+      <c r="C13" s="167"/>
+      <c r="D13" s="169" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="158"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="158"/>
-      <c r="K13" s="158"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="169"/>
+      <c r="J13" s="169"/>
+      <c r="K13" s="169"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="158" t="s">
+      <c r="C14" s="167"/>
+      <c r="D14" s="169" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="169"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="169"/>
+      <c r="K14" s="169"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="156"/>
-      <c r="D15" s="158" t="s">
+      <c r="C15" s="167"/>
+      <c r="D15" s="169" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="169"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="158" t="str">
+      <c r="C16" s="167"/>
+      <c r="D16" s="169" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="169"/>
+      <c r="G16" s="169"/>
+      <c r="H16" s="169"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="169"/>
+      <c r="K16" s="169"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="158">
+      <c r="C17" s="167"/>
+      <c r="D17" s="169">
         <v>0.4</v>
       </c>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="169"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="169"/>
+      <c r="K17" s="169"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="167" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="156"/>
-      <c r="D18" s="157">
+      <c r="C18" s="167"/>
+      <c r="D18" s="168">
         <v>45365</v>
       </c>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="157"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -18495,16 +18495,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="159"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="160"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -22332,6 +22332,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -22348,10 +22352,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="between">
@@ -22437,32 +22437,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -22478,12 +22478,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="155"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="166"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -22491,12 +22491,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="155"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="166"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -22504,12 +22504,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="155"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="166"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -22517,12 +22517,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="155"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="166"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -22530,12 +22530,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="155"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -22583,117 +22583,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="167" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="158" t="str">
+      <c r="C13" s="167"/>
+      <c r="D13" s="169" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="158"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="158"/>
-      <c r="K13" s="158"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="169"/>
+      <c r="J13" s="169"/>
+      <c r="K13" s="169"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="158" t="str">
+      <c r="C14" s="167"/>
+      <c r="D14" s="169" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="169"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="169"/>
+      <c r="K14" s="169"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="156"/>
-      <c r="D15" s="158" t="str">
+      <c r="C15" s="167"/>
+      <c r="D15" s="169" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="169"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="158" t="str">
+      <c r="C16" s="167"/>
+      <c r="D16" s="169" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="169"/>
+      <c r="G16" s="169"/>
+      <c r="H16" s="169"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="169"/>
+      <c r="K16" s="169"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="158">
+      <c r="C17" s="167"/>
+      <c r="D17" s="169">
         <f>Gap30deg!D17</f>
         <v>0.4</v>
       </c>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="169"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="169"/>
+      <c r="K17" s="169"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="167" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="156"/>
-      <c r="D18" s="157">
+      <c r="C18" s="167"/>
+      <c r="D18" s="168">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="157"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -22881,16 +22881,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="159"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="160"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -26719,6 +26719,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -26732,13 +26739,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="between">
@@ -26824,32 +26824,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -26865,12 +26865,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="155"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="166"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -26878,12 +26878,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="155"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="166"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -26891,12 +26891,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="155"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="166"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -26904,12 +26904,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="155"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="166"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -26917,12 +26917,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="155"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -26970,117 +26970,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="167" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="158" t="str">
+      <c r="C13" s="167"/>
+      <c r="D13" s="169" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="158"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="158"/>
-      <c r="K13" s="158"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="169"/>
+      <c r="J13" s="169"/>
+      <c r="K13" s="169"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="158" t="str">
+      <c r="C14" s="167"/>
+      <c r="D14" s="169" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="169"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="169"/>
+      <c r="K14" s="169"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="156"/>
-      <c r="D15" s="158" t="str">
+      <c r="C15" s="167"/>
+      <c r="D15" s="169" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="169"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="158" t="str">
+      <c r="C16" s="167"/>
+      <c r="D16" s="169" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="169"/>
+      <c r="G16" s="169"/>
+      <c r="H16" s="169"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="169"/>
+      <c r="K16" s="169"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="158">
+      <c r="C17" s="167"/>
+      <c r="D17" s="169">
         <f>Gap30deg!D17</f>
         <v>0.4</v>
       </c>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="169"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="169"/>
+      <c r="K17" s="169"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="167" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="156"/>
-      <c r="D18" s="157">
+      <c r="C18" s="167"/>
+      <c r="D18" s="168">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="157"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -27268,16 +27268,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="159"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="160"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -31106,6 +31106,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -31119,13 +31126,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="between">
@@ -31211,32 +31211,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -31252,12 +31252,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="153"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
-      <c r="E5" s="154"/>
-      <c r="F5" s="154"/>
-      <c r="G5" s="155"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="165"/>
+      <c r="D5" s="165"/>
+      <c r="E5" s="165"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="166"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -31265,12 +31265,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="153"/>
-      <c r="C6" s="154"/>
-      <c r="D6" s="154"/>
-      <c r="E6" s="154"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="155"/>
+      <c r="B6" s="164"/>
+      <c r="C6" s="165"/>
+      <c r="D6" s="165"/>
+      <c r="E6" s="165"/>
+      <c r="F6" s="165"/>
+      <c r="G6" s="166"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -31278,12 +31278,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="153"/>
-      <c r="C7" s="154"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="154"/>
-      <c r="F7" s="154"/>
-      <c r="G7" s="155"/>
+      <c r="B7" s="164"/>
+      <c r="C7" s="165"/>
+      <c r="D7" s="165"/>
+      <c r="E7" s="165"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="166"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -31291,12 +31291,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="154"/>
-      <c r="E8" s="154"/>
-      <c r="F8" s="154"/>
-      <c r="G8" s="155"/>
+      <c r="B8" s="164"/>
+      <c r="C8" s="165"/>
+      <c r="D8" s="165"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="166"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -31304,12 +31304,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="153"/>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="155"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -31357,117 +31357,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="156" t="s">
+      <c r="B13" s="167" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="158" t="str">
+      <c r="C13" s="167"/>
+      <c r="D13" s="169" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="158"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="158"/>
-      <c r="K13" s="158"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+      <c r="I13" s="169"/>
+      <c r="J13" s="169"/>
+      <c r="K13" s="169"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="167" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="158" t="str">
+      <c r="C14" s="167"/>
+      <c r="D14" s="169" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="158"/>
-      <c r="F14" s="158"/>
-      <c r="G14" s="158"/>
-      <c r="H14" s="158"/>
-      <c r="I14" s="158"/>
-      <c r="J14" s="158"/>
-      <c r="K14" s="158"/>
+      <c r="E14" s="169"/>
+      <c r="F14" s="169"/>
+      <c r="G14" s="169"/>
+      <c r="H14" s="169"/>
+      <c r="I14" s="169"/>
+      <c r="J14" s="169"/>
+      <c r="K14" s="169"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="156"/>
-      <c r="D15" s="158" t="str">
+      <c r="C15" s="167"/>
+      <c r="D15" s="169" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="169"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="156" t="s">
+      <c r="B16" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="158" t="str">
+      <c r="C16" s="167"/>
+      <c r="D16" s="169" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
+      <c r="E16" s="169"/>
+      <c r="F16" s="169"/>
+      <c r="G16" s="169"/>
+      <c r="H16" s="169"/>
+      <c r="I16" s="169"/>
+      <c r="J16" s="169"/>
+      <c r="K16" s="169"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="156" t="s">
+      <c r="B17" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="156"/>
-      <c r="D17" s="158">
+      <c r="C17" s="167"/>
+      <c r="D17" s="169">
         <f>Gap30deg!D17</f>
         <v>0.4</v>
       </c>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
+      <c r="E17" s="169"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="169"/>
+      <c r="I17" s="169"/>
+      <c r="J17" s="169"/>
+      <c r="K17" s="169"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="156" t="s">
+      <c r="B18" s="167" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="156"/>
-      <c r="D18" s="157">
+      <c r="C18" s="167"/>
+      <c r="D18" s="168">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="157"/>
+      <c r="E18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="G18" s="168"/>
+      <c r="H18" s="168"/>
+      <c r="I18" s="168"/>
+      <c r="J18" s="168"/>
+      <c r="K18" s="168"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -31655,16 +31655,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="162"/>
-      <c r="C28" s="163"/>
-      <c r="D28" s="163"/>
-      <c r="E28" s="163"/>
-      <c r="F28" s="163"/>
-      <c r="G28" s="163"/>
-      <c r="H28" s="163"/>
-      <c r="I28" s="163"/>
-      <c r="J28" s="163"/>
-      <c r="K28" s="164"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="159"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="160"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -35493,6 +35493,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -35506,13 +35513,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="between">
@@ -35549,8 +35549,8 @@
   <dimension ref="B2:Q106"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="26" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <pane ySplit="26" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G105" sqref="G105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -38925,970 +38925,970 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="8" spans="10:13">
-      <c r="J8" s="165"/>
-      <c r="K8" s="165"/>
-      <c r="L8" s="165"/>
-      <c r="M8" s="165"/>
+      <c r="J8" s="153"/>
+      <c r="K8" s="153"/>
+      <c r="L8" s="153"/>
+      <c r="M8" s="153"/>
     </row>
     <row r="9" spans="10:13">
-      <c r="J9" s="166">
+      <c r="J9" s="154">
         <v>153.69999999999999</v>
       </c>
-      <c r="K9" s="166">
+      <c r="K9" s="154">
         <v>153.69999999999999</v>
       </c>
-      <c r="L9" s="166">
+      <c r="L9" s="154">
         <v>153.69999999999999</v>
       </c>
-      <c r="M9" s="166">
+      <c r="M9" s="154">
         <v>153.69999999999999</v>
       </c>
     </row>
     <row r="10" spans="10:13">
-      <c r="J10" s="166">
+      <c r="J10" s="154">
         <v>900</v>
       </c>
-      <c r="K10" s="166">
+      <c r="K10" s="154">
         <v>900</v>
       </c>
-      <c r="L10" s="166">
+      <c r="L10" s="154">
         <v>900</v>
       </c>
-      <c r="M10" s="166">
+      <c r="M10" s="154">
         <v>900</v>
       </c>
     </row>
     <row r="11" spans="10:13">
-      <c r="J11" s="166">
+      <c r="J11" s="154">
         <v>4344.1000000000004</v>
       </c>
-      <c r="K11" s="166">
+      <c r="K11" s="154">
         <v>4344.1000000000004</v>
       </c>
-      <c r="L11" s="166">
+      <c r="L11" s="154">
         <v>4344.1000000000004</v>
       </c>
-      <c r="M11" s="166">
+      <c r="M11" s="154">
         <v>4344.1000000000004</v>
       </c>
     </row>
     <row r="12" spans="10:13">
-      <c r="J12" s="166">
+      <c r="J12" s="154">
         <v>2876</v>
       </c>
-      <c r="K12" s="166">
+      <c r="K12" s="154">
         <v>2876</v>
       </c>
-      <c r="L12" s="166">
+      <c r="L12" s="154">
         <v>2876</v>
       </c>
-      <c r="M12" s="166">
+      <c r="M12" s="154">
         <v>2876</v>
       </c>
     </row>
     <row r="13" spans="10:13">
-      <c r="J13" s="166">
+      <c r="J13" s="154">
         <v>3144.2</v>
       </c>
-      <c r="K13" s="166">
+      <c r="K13" s="154">
         <v>3144.2</v>
       </c>
-      <c r="L13" s="166">
+      <c r="L13" s="154">
         <v>3144.2</v>
       </c>
-      <c r="M13" s="166">
+      <c r="M13" s="154">
         <v>3144.2</v>
       </c>
     </row>
     <row r="14" spans="10:13">
-      <c r="J14" s="166">
+      <c r="J14" s="154">
         <v>0.03</v>
       </c>
-      <c r="K14" s="166">
+      <c r="K14" s="154">
         <v>0.03</v>
       </c>
-      <c r="L14" s="166">
+      <c r="L14" s="154">
         <v>0.03</v>
       </c>
-      <c r="M14" s="166">
+      <c r="M14" s="154">
         <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="10:13">
-      <c r="J15" s="166">
+      <c r="J15" s="154">
         <v>3074.8</v>
       </c>
-      <c r="K15" s="166">
+      <c r="K15" s="154">
         <v>3074.8</v>
       </c>
-      <c r="L15" s="166">
+      <c r="L15" s="154">
         <v>3074.8</v>
       </c>
-      <c r="M15" s="166">
+      <c r="M15" s="154">
         <v>3074.8</v>
       </c>
     </row>
     <row r="16" spans="10:13">
-      <c r="J16" s="167">
+      <c r="J16" s="155">
         <v>2466</v>
       </c>
-      <c r="K16" s="167">
+      <c r="K16" s="155">
         <v>2466</v>
       </c>
-      <c r="L16" s="167">
+      <c r="L16" s="155">
         <v>2466</v>
       </c>
-      <c r="M16" s="167">
+      <c r="M16" s="155">
         <v>2466</v>
       </c>
     </row>
     <row r="17" spans="10:13">
-      <c r="J17" s="168">
+      <c r="J17" s="156">
         <v>5.8500000000000005E-10</v>
       </c>
-      <c r="K17" s="168">
+      <c r="K17" s="156">
         <v>5.8500000000000005E-10</v>
       </c>
-      <c r="L17" s="168">
+      <c r="L17" s="156">
         <v>5.8500000000000005E-10</v>
       </c>
-      <c r="M17" s="168">
+      <c r="M17" s="156">
         <v>5.8500000000000005E-10</v>
       </c>
     </row>
     <row r="18" spans="10:13">
-      <c r="J18" s="168">
+      <c r="J18" s="156">
         <v>9.7000000000000001E-11</v>
       </c>
-      <c r="K18" s="168">
+      <c r="K18" s="156">
         <v>9.7000000000000001E-11</v>
       </c>
-      <c r="L18" s="168">
+      <c r="L18" s="156">
         <v>9.7000000000000001E-11</v>
       </c>
-      <c r="M18" s="168">
+      <c r="M18" s="156">
         <v>9.7000000000000001E-11</v>
       </c>
     </row>
     <row r="19" spans="10:13">
-      <c r="J19" s="166">
+      <c r="J19" s="154">
         <v>0.14199999999999999</v>
       </c>
-      <c r="K19" s="166">
+      <c r="K19" s="154">
         <v>0.14199999999999999</v>
       </c>
-      <c r="L19" s="166">
+      <c r="L19" s="154">
         <v>0.14199999999999999</v>
       </c>
-      <c r="M19" s="166">
+      <c r="M19" s="154">
         <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="20" spans="10:13">
-      <c r="J20" s="166">
+      <c r="J20" s="154">
         <v>48.86</v>
       </c>
-      <c r="K20" s="166">
+      <c r="K20" s="154">
         <v>48.86</v>
       </c>
-      <c r="L20" s="166">
+      <c r="L20" s="154">
         <v>48.86</v>
       </c>
-      <c r="M20" s="166">
+      <c r="M20" s="154">
         <v>48.86</v>
       </c>
     </row>
     <row r="21" spans="10:13">
-      <c r="J21" s="166">
+      <c r="J21" s="154">
         <v>200</v>
       </c>
-      <c r="K21" s="166">
+      <c r="K21" s="154">
         <v>200</v>
       </c>
-      <c r="L21" s="166">
+      <c r="L21" s="154">
         <v>200</v>
       </c>
-      <c r="M21" s="166">
+      <c r="M21" s="154">
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="10:13">
-      <c r="J22" s="166">
+      <c r="J22" s="154">
         <v>33.299999999999997</v>
       </c>
-      <c r="K22" s="166">
+      <c r="K22" s="154">
         <v>33.299999999999997</v>
       </c>
-      <c r="L22" s="166">
+      <c r="L22" s="154">
         <v>33.299999999999997</v>
       </c>
-      <c r="M22" s="166">
+      <c r="M22" s="154">
         <v>33.299999999999997</v>
       </c>
     </row>
     <row r="23" spans="10:13">
-      <c r="J23" s="166">
+      <c r="J23" s="154">
         <v>3323</v>
       </c>
-      <c r="K23" s="166">
+      <c r="K23" s="154">
         <v>3323</v>
       </c>
-      <c r="L23" s="166">
+      <c r="L23" s="154">
         <v>3323</v>
       </c>
-      <c r="M23" s="166">
+      <c r="M23" s="154">
         <v>3323</v>
       </c>
     </row>
     <row r="24" spans="10:13">
-      <c r="J24" s="166">
+      <c r="J24" s="154">
         <v>311.2</v>
       </c>
-      <c r="K24" s="166">
+      <c r="K24" s="154">
         <v>311.2</v>
       </c>
-      <c r="L24" s="166">
+      <c r="L24" s="154">
         <v>311.2</v>
       </c>
-      <c r="M24" s="166">
+      <c r="M24" s="154">
         <v>311.2</v>
       </c>
     </row>
     <row r="25" spans="10:13">
-      <c r="J25" s="166">
+      <c r="J25" s="154">
         <v>311.2</v>
       </c>
-      <c r="K25" s="166">
+      <c r="K25" s="154">
         <v>311.2</v>
       </c>
-      <c r="L25" s="166">
+      <c r="L25" s="154">
         <v>311.2</v>
       </c>
-      <c r="M25" s="166">
+      <c r="M25" s="154">
         <v>311.2</v>
       </c>
     </row>
     <row r="26" spans="10:13">
-      <c r="J26" s="166">
+      <c r="J26" s="154">
         <v>-303.89999999999998</v>
       </c>
-      <c r="K26" s="166">
+      <c r="K26" s="154">
         <v>-303.89999999999998</v>
       </c>
-      <c r="L26" s="166">
+      <c r="L26" s="154">
         <v>-303.89999999999998</v>
       </c>
-      <c r="M26" s="166">
+      <c r="M26" s="154">
         <v>-303.89999999999998</v>
       </c>
     </row>
     <row r="27" spans="10:13">
-      <c r="J27" s="166">
+      <c r="J27" s="154">
         <v>3237</v>
       </c>
-      <c r="K27" s="166">
+      <c r="K27" s="154">
         <v>3332</v>
       </c>
-      <c r="L27" s="166">
+      <c r="L27" s="154">
         <v>3376</v>
       </c>
-      <c r="M27" s="166">
+      <c r="M27" s="154">
         <v>3404</v>
       </c>
     </row>
     <row r="28" spans="10:13">
-      <c r="J28" s="165"/>
-      <c r="K28" s="165"/>
-      <c r="L28" s="165"/>
-      <c r="M28" s="165"/>
+      <c r="J28" s="153"/>
+      <c r="K28" s="153"/>
+      <c r="L28" s="153"/>
+      <c r="M28" s="153"/>
     </row>
     <row r="29" spans="10:13">
-      <c r="J29" s="166">
+      <c r="J29" s="154">
         <v>30</v>
       </c>
-      <c r="K29" s="166">
+      <c r="K29" s="154">
         <v>60</v>
       </c>
-      <c r="L29" s="166">
+      <c r="L29" s="154">
         <v>90</v>
       </c>
-      <c r="M29" s="166">
+      <c r="M29" s="154">
         <v>120</v>
       </c>
     </row>
     <row r="30" spans="10:13">
-      <c r="J30" s="166">
+      <c r="J30" s="154">
         <v>1.9630000000000001</v>
       </c>
-      <c r="K30" s="166">
+      <c r="K30" s="154">
         <v>3.927</v>
       </c>
-      <c r="L30" s="166">
+      <c r="L30" s="154">
         <v>5.89</v>
       </c>
-      <c r="M30" s="166">
+      <c r="M30" s="154">
         <v>7.8540000000000001</v>
       </c>
     </row>
     <row r="31" spans="10:13">
-      <c r="J31" s="166">
+      <c r="J31" s="154">
         <v>7.5</v>
       </c>
-      <c r="K31" s="166">
+      <c r="K31" s="154">
         <v>7.5</v>
       </c>
-      <c r="L31" s="166">
+      <c r="L31" s="154">
         <v>7.5</v>
       </c>
-      <c r="M31" s="166">
+      <c r="M31" s="154">
         <v>7.5</v>
       </c>
     </row>
     <row r="32" spans="10:13">
-      <c r="J32" s="166">
+      <c r="J32" s="154">
         <v>1.4</v>
       </c>
-      <c r="K32" s="166">
+      <c r="K32" s="154">
         <v>1.4</v>
       </c>
-      <c r="L32" s="166">
+      <c r="L32" s="154">
         <v>1.4</v>
       </c>
-      <c r="M32" s="166">
+      <c r="M32" s="154">
         <v>1.4</v>
       </c>
     </row>
     <row r="33" spans="10:13">
-      <c r="J33" s="166">
+      <c r="J33" s="154">
         <v>0.28799999999999998</v>
       </c>
-      <c r="K33" s="166">
+      <c r="K33" s="154">
         <v>0.74299999999999999</v>
       </c>
-      <c r="L33" s="166">
+      <c r="L33" s="154">
         <v>1.3640000000000001</v>
       </c>
-      <c r="M33" s="166">
+      <c r="M33" s="154">
         <v>2.153</v>
       </c>
     </row>
     <row r="34" spans="10:13">
-      <c r="J34" s="166">
+      <c r="J34" s="154">
         <v>1.216</v>
       </c>
-      <c r="K34" s="166">
+      <c r="K34" s="154">
         <v>0.63600000000000001</v>
       </c>
-      <c r="L34" s="166">
+      <c r="L34" s="154">
         <v>0.499</v>
       </c>
-      <c r="M34" s="166">
+      <c r="M34" s="154">
         <v>0.44400000000000001</v>
       </c>
     </row>
     <row r="35" spans="10:13">
-      <c r="J35" s="166">
+      <c r="J35" s="154">
         <v>1.9630000000000001</v>
       </c>
-      <c r="K35" s="166">
+      <c r="K35" s="154">
         <v>1.9630000000000001</v>
       </c>
-      <c r="L35" s="166">
+      <c r="L35" s="154">
         <v>1.9630000000000001</v>
       </c>
-      <c r="M35" s="166">
+      <c r="M35" s="154">
         <v>1.9630000000000001</v>
       </c>
     </row>
     <row r="36" spans="10:13">
-      <c r="J36" s="166">
+      <c r="J36" s="154">
         <v>1.962</v>
       </c>
-      <c r="K36" s="166">
+      <c r="K36" s="154">
         <v>1.962</v>
       </c>
-      <c r="L36" s="166">
+      <c r="L36" s="154">
         <v>1.962</v>
       </c>
-      <c r="M36" s="166">
+      <c r="M36" s="154">
         <v>1.962</v>
       </c>
     </row>
     <row r="37" spans="10:13">
-      <c r="J37" s="166">
+      <c r="J37" s="154">
         <v>2.9430000000000001</v>
       </c>
-      <c r="K37" s="166">
+      <c r="K37" s="154">
         <v>2.9430000000000001</v>
       </c>
-      <c r="L37" s="166">
+      <c r="L37" s="154">
         <v>2.9430000000000001</v>
       </c>
-      <c r="M37" s="166">
+      <c r="M37" s="154">
         <v>2.9430000000000001</v>
       </c>
     </row>
     <row r="38" spans="10:13">
-      <c r="J38" s="166">
+      <c r="J38" s="154">
         <v>0.95299999999999996</v>
       </c>
-      <c r="K38" s="166">
+      <c r="K38" s="154">
         <v>0.58299999999999996</v>
       </c>
-      <c r="L38" s="166">
+      <c r="L38" s="154">
         <v>0.47199999999999998</v>
       </c>
-      <c r="M38" s="166">
+      <c r="M38" s="154">
         <v>0.42399999999999999</v>
       </c>
     </row>
     <row r="39" spans="10:13">
-      <c r="J39" s="166">
+      <c r="J39" s="154">
         <v>-1.7</v>
       </c>
-      <c r="K39" s="166">
+      <c r="K39" s="154">
         <v>-0.46700000000000003</v>
       </c>
-      <c r="L39" s="166">
+      <c r="L39" s="154">
         <v>0.19900000000000001</v>
       </c>
-      <c r="M39" s="166">
+      <c r="M39" s="154">
         <v>0.67700000000000005</v>
       </c>
     </row>
     <row r="40" spans="10:13">
-      <c r="J40" s="166">
+      <c r="J40" s="154">
         <v>-0.13200000000000001</v>
       </c>
-      <c r="K40" s="166">
+      <c r="K40" s="154">
         <v>0.49099999999999999</v>
       </c>
-      <c r="L40" s="166">
+      <c r="L40" s="154">
         <v>0.97599999999999998</v>
       </c>
-      <c r="M40" s="166">
+      <c r="M40" s="154">
         <v>1.375</v>
       </c>
     </row>
     <row r="41" spans="10:13">
-      <c r="J41" s="166">
+      <c r="J41" s="154">
         <v>0.876</v>
       </c>
-      <c r="K41" s="166">
+      <c r="K41" s="154">
         <v>1.6339999999999999</v>
       </c>
-      <c r="L41" s="166">
+      <c r="L41" s="154">
         <v>2.653</v>
       </c>
-      <c r="M41" s="166">
+      <c r="M41" s="154">
         <v>3.9550000000000001</v>
       </c>
     </row>
     <row r="42" spans="10:13">
-      <c r="J42" s="166">
+      <c r="J42" s="154">
         <v>0.876</v>
       </c>
-      <c r="K42" s="166">
+      <c r="K42" s="154">
         <v>1.6339999999999999</v>
       </c>
-      <c r="L42" s="166">
+      <c r="L42" s="154">
         <v>2.653</v>
       </c>
-      <c r="M42" s="166">
+      <c r="M42" s="154">
         <v>3.9550000000000001</v>
       </c>
     </row>
     <row r="43" spans="10:13">
-      <c r="J43" s="169"/>
-      <c r="K43" s="169"/>
-      <c r="L43" s="169"/>
-      <c r="M43" s="169"/>
+      <c r="J43" s="157"/>
+      <c r="K43" s="157"/>
+      <c r="L43" s="157"/>
+      <c r="M43" s="157"/>
     </row>
     <row r="44" spans="10:13">
-      <c r="J44" s="169"/>
-      <c r="K44" s="169"/>
-      <c r="L44" s="169"/>
-      <c r="M44" s="169"/>
+      <c r="J44" s="157"/>
+      <c r="K44" s="157"/>
+      <c r="L44" s="157"/>
+      <c r="M44" s="157"/>
     </row>
     <row r="45" spans="10:13">
-      <c r="J45" s="165"/>
-      <c r="K45" s="165"/>
-      <c r="L45" s="165"/>
-      <c r="M45" s="165"/>
+      <c r="J45" s="153"/>
+      <c r="K45" s="153"/>
+      <c r="L45" s="153"/>
+      <c r="M45" s="153"/>
     </row>
     <row r="46" spans="10:13">
-      <c r="J46" s="165"/>
-      <c r="K46" s="165"/>
-      <c r="L46" s="165"/>
-      <c r="M46" s="165"/>
+      <c r="J46" s="153"/>
+      <c r="K46" s="153"/>
+      <c r="L46" s="153"/>
+      <c r="M46" s="153"/>
     </row>
     <row r="47" spans="10:13">
-      <c r="J47" s="169"/>
-      <c r="K47" s="169"/>
-      <c r="L47" s="169"/>
-      <c r="M47" s="169"/>
+      <c r="J47" s="157"/>
+      <c r="K47" s="157"/>
+      <c r="L47" s="157"/>
+      <c r="M47" s="157"/>
     </row>
     <row r="48" spans="10:13">
-      <c r="J48" s="166">
+      <c r="J48" s="154">
         <v>1234.8</v>
       </c>
-      <c r="K48" s="166">
+      <c r="K48" s="154">
         <v>806.6</v>
       </c>
-      <c r="L48" s="166">
+      <c r="L48" s="154">
         <v>713.5</v>
       </c>
-      <c r="M48" s="166">
+      <c r="M48" s="154">
         <v>682.4</v>
       </c>
     </row>
     <row r="49" spans="10:13">
-      <c r="J49" s="166">
+      <c r="J49" s="154">
         <v>37149</v>
       </c>
-      <c r="K49" s="166">
+      <c r="K49" s="154">
         <v>37149</v>
       </c>
-      <c r="L49" s="166">
+      <c r="L49" s="154">
         <v>37149</v>
       </c>
-      <c r="M49" s="166">
+      <c r="M49" s="154">
         <v>37149</v>
       </c>
     </row>
     <row r="50" spans="10:13">
-      <c r="J50" s="168">
+      <c r="J50" s="156">
         <v>124000000</v>
       </c>
-      <c r="K50" s="168">
+      <c r="K50" s="156">
         <v>124000000</v>
       </c>
-      <c r="L50" s="168">
+      <c r="L50" s="156">
         <v>124000000</v>
       </c>
-      <c r="M50" s="168">
+      <c r="M50" s="156">
         <v>124000000</v>
       </c>
     </row>
     <row r="51" spans="10:13">
-      <c r="J51" s="166">
+      <c r="J51" s="154">
         <v>87000</v>
       </c>
-      <c r="K51" s="166">
+      <c r="K51" s="154">
         <v>87000</v>
       </c>
-      <c r="L51" s="166">
+      <c r="L51" s="154">
         <v>87000</v>
       </c>
-      <c r="M51" s="166">
+      <c r="M51" s="154">
         <v>87000</v>
       </c>
     </row>
     <row r="52" spans="10:13">
-      <c r="J52" s="168">
+      <c r="J52" s="156">
         <v>290000000</v>
       </c>
-      <c r="K52" s="168">
+      <c r="K52" s="156">
         <v>290000000</v>
       </c>
-      <c r="L52" s="168">
+      <c r="L52" s="156">
         <v>290000000</v>
       </c>
-      <c r="M52" s="168">
+      <c r="M52" s="156">
         <v>290000000</v>
       </c>
     </row>
     <row r="53" spans="10:13">
-      <c r="J53" s="166">
+      <c r="J53" s="154">
         <v>14497</v>
       </c>
-      <c r="K53" s="166">
+      <c r="K53" s="154">
         <v>5077</v>
       </c>
-      <c r="L53" s="166">
+      <c r="L53" s="154">
         <v>2767</v>
       </c>
-      <c r="M53" s="166">
+      <c r="M53" s="154">
         <v>1774</v>
       </c>
     </row>
     <row r="54" spans="10:13">
-      <c r="J54" s="166">
+      <c r="J54" s="154">
         <v>4817</v>
       </c>
-      <c r="K54" s="166">
+      <c r="K54" s="154">
         <v>2025</v>
       </c>
-      <c r="L54" s="166">
+      <c r="L54" s="154">
         <v>1073</v>
       </c>
-      <c r="M54" s="166">
+      <c r="M54" s="154">
         <v>608</v>
       </c>
     </row>
     <row r="55" spans="10:13">
-      <c r="J55" s="166">
+      <c r="J55" s="154">
         <v>5169</v>
       </c>
-      <c r="K55" s="166">
+      <c r="K55" s="154">
         <v>2212</v>
       </c>
-      <c r="L55" s="166">
+      <c r="L55" s="154">
         <v>1238</v>
       </c>
-      <c r="M55" s="166">
+      <c r="M55" s="154">
         <v>800</v>
       </c>
     </row>
     <row r="56" spans="10:13">
-      <c r="J56" s="166">
+      <c r="J56" s="154">
         <v>5169</v>
       </c>
-      <c r="K56" s="166">
+      <c r="K56" s="154">
         <v>2212</v>
       </c>
-      <c r="L56" s="166">
+      <c r="L56" s="154">
         <v>1238</v>
       </c>
-      <c r="M56" s="166">
+      <c r="M56" s="154">
         <v>800</v>
       </c>
     </row>
     <row r="57" spans="10:13">
-      <c r="J57" s="166">
+      <c r="J57" s="154">
         <v>1.8</v>
       </c>
-      <c r="K57" s="166">
+      <c r="K57" s="154">
         <v>2.1030000000000002</v>
       </c>
-      <c r="L57" s="166">
+      <c r="L57" s="154">
         <v>2.5049999999999999</v>
       </c>
-      <c r="M57" s="166">
+      <c r="M57" s="154">
         <v>2.9060000000000001</v>
       </c>
     </row>
     <row r="58" spans="10:13">
-      <c r="J58" s="166">
+      <c r="J58" s="154">
         <v>1420.1</v>
       </c>
-      <c r="K58" s="166">
+      <c r="K58" s="154">
         <v>95.8</v>
       </c>
-      <c r="L58" s="166">
+      <c r="L58" s="154">
         <v>19.2</v>
       </c>
-      <c r="M58" s="166">
+      <c r="M58" s="154">
         <v>6.1</v>
       </c>
     </row>
     <row r="59" spans="10:13">
-      <c r="J59" s="165"/>
-      <c r="K59" s="165"/>
-      <c r="L59" s="165"/>
-      <c r="M59" s="165"/>
+      <c r="J59" s="153"/>
+      <c r="K59" s="153"/>
+      <c r="L59" s="153"/>
+      <c r="M59" s="153"/>
     </row>
     <row r="60" spans="10:13">
-      <c r="J60" s="165"/>
-      <c r="K60" s="165"/>
-      <c r="L60" s="165"/>
-      <c r="M60" s="165"/>
+      <c r="J60" s="153"/>
+      <c r="K60" s="153"/>
+      <c r="L60" s="153"/>
+      <c r="M60" s="153"/>
     </row>
     <row r="61" spans="10:13">
-      <c r="J61" s="165"/>
-      <c r="K61" s="165"/>
-      <c r="L61" s="165"/>
-      <c r="M61" s="165"/>
+      <c r="J61" s="153"/>
+      <c r="K61" s="153"/>
+      <c r="L61" s="153"/>
+      <c r="M61" s="153"/>
     </row>
     <row r="62" spans="10:13">
-      <c r="J62" s="166">
+      <c r="J62" s="154">
         <v>1234.8</v>
       </c>
-      <c r="K62" s="166">
+      <c r="K62" s="154">
         <v>806.6</v>
       </c>
-      <c r="L62" s="166">
+      <c r="L62" s="154">
         <v>713.5</v>
       </c>
-      <c r="M62" s="166">
+      <c r="M62" s="154">
         <v>682.4</v>
       </c>
     </row>
     <row r="63" spans="10:13">
-      <c r="J63" s="166">
+      <c r="J63" s="154">
         <v>3595</v>
       </c>
-      <c r="K63" s="166">
+      <c r="K63" s="154">
         <v>3595</v>
       </c>
-      <c r="L63" s="166">
+      <c r="L63" s="154">
         <v>3595</v>
       </c>
-      <c r="M63" s="166">
+      <c r="M63" s="154">
         <v>3595</v>
       </c>
     </row>
     <row r="64" spans="10:13">
-      <c r="J64" s="166">
+      <c r="J64" s="154">
         <v>2068.3000000000002</v>
       </c>
-      <c r="K64" s="166">
+      <c r="K64" s="154">
         <v>2068.3000000000002</v>
       </c>
-      <c r="L64" s="166">
+      <c r="L64" s="154">
         <v>2068.3000000000002</v>
       </c>
-      <c r="M64" s="166">
+      <c r="M64" s="154">
         <v>2068.3000000000002</v>
       </c>
     </row>
     <row r="65" spans="10:13">
-      <c r="J65" s="165"/>
-      <c r="K65" s="165"/>
-      <c r="L65" s="165"/>
-      <c r="M65" s="165"/>
+      <c r="J65" s="153"/>
+      <c r="K65" s="153"/>
+      <c r="L65" s="153"/>
+      <c r="M65" s="153"/>
     </row>
     <row r="66" spans="10:13">
-      <c r="J66" s="166">
+      <c r="J66" s="154">
         <v>2.403</v>
       </c>
-      <c r="K66" s="166">
+      <c r="K66" s="154">
         <v>1.345</v>
       </c>
-      <c r="L66" s="166">
+      <c r="L66" s="154">
         <v>1.177</v>
       </c>
-      <c r="M66" s="166">
+      <c r="M66" s="154">
         <v>1.111</v>
       </c>
     </row>
     <row r="67" spans="10:13">
-      <c r="J67" s="166">
+      <c r="J67" s="154">
         <v>194.5</v>
       </c>
-      <c r="K67" s="166">
+      <c r="K67" s="154">
         <v>194.5</v>
       </c>
-      <c r="L67" s="166">
+      <c r="L67" s="154">
         <v>194.5</v>
       </c>
-      <c r="M67" s="166">
+      <c r="M67" s="154">
         <v>194.5</v>
       </c>
     </row>
     <row r="68" spans="10:13">
-      <c r="J68" s="166">
+      <c r="J68" s="154">
         <v>10330.700000000001</v>
       </c>
-      <c r="K68" s="166">
+      <c r="K68" s="154">
         <v>14733.5</v>
       </c>
-      <c r="L68" s="166">
+      <c r="L68" s="154">
         <v>15624</v>
       </c>
-      <c r="M68" s="166">
+      <c r="M68" s="154">
         <v>15916.9</v>
       </c>
     </row>
     <row r="69" spans="10:13">
-      <c r="J69" s="166">
+      <c r="J69" s="154">
         <v>833</v>
       </c>
-      <c r="K69" s="166">
+      <c r="K69" s="154">
         <v>1262</v>
       </c>
-      <c r="L69" s="166">
+      <c r="L69" s="154">
         <v>1355</v>
       </c>
-      <c r="M69" s="166">
+      <c r="M69" s="154">
         <v>1386</v>
       </c>
     </row>
     <row r="70" spans="10:13">
-      <c r="J70" s="166">
+      <c r="J70" s="154">
         <v>0.41499999999999998</v>
       </c>
-      <c r="K70" s="166">
+      <c r="K70" s="154">
         <v>0.44</v>
       </c>
-      <c r="L70" s="166">
+      <c r="L70" s="154">
         <v>0.44600000000000001</v>
       </c>
-      <c r="M70" s="166">
+      <c r="M70" s="154">
         <v>0.44800000000000001</v>
       </c>
     </row>
     <row r="71" spans="10:13">
-      <c r="J71" s="165"/>
-      <c r="K71" s="165"/>
-      <c r="L71" s="165"/>
-      <c r="M71" s="165"/>
+      <c r="J71" s="153"/>
+      <c r="K71" s="153"/>
+      <c r="L71" s="153"/>
+      <c r="M71" s="153"/>
     </row>
     <row r="72" spans="10:13">
-      <c r="J72" s="166">
+      <c r="J72" s="154">
         <v>14795</v>
       </c>
-      <c r="K72" s="166">
+      <c r="K72" s="154">
         <v>14795</v>
       </c>
-      <c r="L72" s="166">
+      <c r="L72" s="154">
         <v>14795</v>
       </c>
-      <c r="M72" s="166">
+      <c r="M72" s="154">
         <v>14795</v>
       </c>
     </row>
     <row r="73" spans="10:13">
-      <c r="J73" s="166">
+      <c r="J73" s="154">
         <v>-123.3</v>
       </c>
-      <c r="K73" s="166">
+      <c r="K73" s="154">
         <v>-123.3</v>
       </c>
-      <c r="L73" s="166">
+      <c r="L73" s="154">
         <v>-123.3</v>
       </c>
-      <c r="M73" s="166">
+      <c r="M73" s="154">
         <v>-123.3</v>
       </c>
     </row>
     <row r="74" spans="10:13">
-      <c r="J74" s="165"/>
-      <c r="K74" s="165"/>
-      <c r="L74" s="165"/>
-      <c r="M74" s="165"/>
+      <c r="J74" s="153"/>
+      <c r="K74" s="153"/>
+      <c r="L74" s="153"/>
+      <c r="M74" s="153"/>
     </row>
     <row r="75" spans="10:13">
-      <c r="J75" s="166">
+      <c r="J75" s="154">
         <v>-1358.1</v>
       </c>
-      <c r="K75" s="166">
+      <c r="K75" s="154">
         <v>-929.9</v>
       </c>
-      <c r="L75" s="166">
+      <c r="L75" s="154">
         <v>-836.8</v>
       </c>
-      <c r="M75" s="166">
+      <c r="M75" s="154">
         <v>-805.7</v>
       </c>
     </row>
     <row r="76" spans="10:13">
-      <c r="J76" s="166">
+      <c r="J76" s="154">
         <v>0.106</v>
       </c>
-      <c r="K76" s="166">
+      <c r="K76" s="154">
         <v>0.1</v>
       </c>
-      <c r="L76" s="166">
+      <c r="L76" s="154">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="M76" s="166">
+      <c r="M76" s="154">
         <v>9.4E-2</v>
       </c>
     </row>
     <row r="77" spans="10:13">
-      <c r="J77" s="166">
+      <c r="J77" s="154">
         <v>2810.3</v>
       </c>
-      <c r="K77" s="166">
+      <c r="K77" s="154">
         <v>2835.72</v>
       </c>
-      <c r="L77" s="166">
+      <c r="L77" s="154">
         <v>2841.56</v>
       </c>
-      <c r="M77" s="166">
+      <c r="M77" s="154">
         <v>2843.91</v>
       </c>
     </row>
     <row r="78" spans="10:13">
-      <c r="J78" s="165"/>
-      <c r="K78" s="165"/>
-      <c r="L78" s="165"/>
-      <c r="M78" s="165"/>
+      <c r="J78" s="153"/>
+      <c r="K78" s="153"/>
+      <c r="L78" s="153"/>
+      <c r="M78" s="153"/>
     </row>
     <row r="79" spans="10:13">
-      <c r="J79" s="165"/>
-      <c r="K79" s="165"/>
-      <c r="L79" s="165"/>
-      <c r="M79" s="165"/>
+      <c r="J79" s="153"/>
+      <c r="K79" s="153"/>
+      <c r="L79" s="153"/>
+      <c r="M79" s="153"/>
     </row>
     <row r="80" spans="10:13">
-      <c r="J80" s="169"/>
-      <c r="K80" s="169"/>
-      <c r="L80" s="169"/>
-      <c r="M80" s="169"/>
+      <c r="J80" s="157"/>
+      <c r="K80" s="157"/>
+      <c r="L80" s="157"/>
+      <c r="M80" s="157"/>
     </row>
     <row r="81" spans="10:13">
-      <c r="J81" s="166">
+      <c r="J81" s="154">
         <v>112.8</v>
       </c>
-      <c r="K81" s="166">
+      <c r="K81" s="154">
         <v>112.8</v>
       </c>
-      <c r="L81" s="166">
+      <c r="L81" s="154">
         <v>112.8</v>
       </c>
-      <c r="M81" s="166">
+      <c r="M81" s="154">
         <v>112.8</v>
       </c>
     </row>
     <row r="82" spans="10:13">
-      <c r="J82" s="168">
+      <c r="J82" s="156">
         <v>1.6600000000000001E-9</v>
       </c>
-      <c r="K82" s="168">
+      <c r="K82" s="156">
         <v>1.6600000000000001E-9</v>
       </c>
-      <c r="L82" s="168">
+      <c r="L82" s="156">
         <v>1.6600000000000001E-9</v>
       </c>
-      <c r="M82" s="168">
+      <c r="M82" s="156">
         <v>1.6600000000000001E-9</v>
       </c>
     </row>
     <row r="83" spans="10:13">
-      <c r="J83" s="169"/>
-      <c r="K83" s="169"/>
-      <c r="L83" s="169"/>
-      <c r="M83" s="169"/>
+      <c r="J83" s="157"/>
+      <c r="K83" s="157"/>
+      <c r="L83" s="157"/>
+      <c r="M83" s="157"/>
     </row>
     <row r="84" spans="10:13">
-      <c r="J84" s="169"/>
-      <c r="K84" s="169"/>
-      <c r="L84" s="169"/>
-      <c r="M84" s="169"/>
+      <c r="J84" s="157"/>
+      <c r="K84" s="157"/>
+      <c r="L84" s="157"/>
+      <c r="M84" s="157"/>
     </row>
     <row r="85" spans="10:13">
-      <c r="J85" s="169"/>
-      <c r="K85" s="169"/>
-      <c r="L85" s="169"/>
-      <c r="M85" s="169"/>
+      <c r="J85" s="157"/>
+      <c r="K85" s="157"/>
+      <c r="L85" s="157"/>
+      <c r="M85" s="157"/>
     </row>
     <row r="86" spans="10:13">
-      <c r="J86" s="166">
+      <c r="J86" s="154">
         <v>0.45200000000000001</v>
       </c>
-      <c r="K86" s="166">
+      <c r="K86" s="154">
         <v>0.52600000000000002</v>
       </c>
-      <c r="L86" s="166">
+      <c r="L86" s="154">
         <v>0.54600000000000004</v>
       </c>
-      <c r="M86" s="166">
+      <c r="M86" s="154">
         <v>0.55300000000000005</v>
       </c>
     </row>
     <row r="87" spans="10:13">
-      <c r="J87" s="166">
+      <c r="J87" s="154">
         <v>-319.14</v>
       </c>
-      <c r="K87" s="166">
+      <c r="K87" s="154">
         <v>-266.89999999999998</v>
       </c>
-      <c r="L87" s="166">
+      <c r="L87" s="154">
         <v>-253.98</v>
       </c>
-      <c r="M87" s="166">
+      <c r="M87" s="154">
         <v>-249.73</v>
       </c>
     </row>
@@ -39898,6 +39898,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -40150,38 +40167,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -40204,9 +40193,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
flangesegments: added validation for failure mode B in L-Flange Segment
</commit_message>
<xml_diff>
--- a/tests/validation-BnB_3p228mm/BnB_3p228mm-Results.xlsx
+++ b/tests/validation-BnB_3p228mm/BnB_3p228mm-Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcellob\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation-BnB_3p228mm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\tests\validation-BnB_3p228mm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE529AF-E750-44F1-9ACA-17E351F3248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D22A68C-7A56-45A3-B070-658BC21FB5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -4676,6 +4676,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4693,24 +4711,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5339,25 +5339,25 @@
                   <c:v>-17.127219714134611</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-7.0896214729580294</c:v>
+                  <c:v>-7.0896214729580223</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.046558991994516</c:v>
+                  <c:v>9.0465589919945231</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>26.06635477055708</c:v>
+                  <c:v>26.066354770557087</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>43.969765862729538</c:v>
+                  <c:v>43.969765862729545</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>62.756792268512129</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>82.42743398790472</c:v>
+                  <c:v>82.427433987904735</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>102.98169102090735</c:v>
+                  <c:v>102.98169102090736</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>124.41956336751997</c:v>
@@ -5372,7 +5372,7 @@
                   <c:v>194.03487228901781</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>219.00720589007051</c:v>
+                  <c:v>219.00720589007054</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>244.86315480473326</c:v>
@@ -5620,7 +5620,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5658,7 +5658,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -5742,7 +5742,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5780,7 +5780,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -5823,7 +5823,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6577,7 +6577,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6615,7 +6615,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -6700,7 +6700,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6738,7 +6738,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -6781,7 +6781,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7535,7 +7535,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7573,7 +7573,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -7657,7 +7657,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7695,7 +7695,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -7738,7 +7738,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8492,7 +8492,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8530,7 +8530,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -8615,7 +8615,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -8653,7 +8653,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -8696,7 +8696,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9450,7 +9450,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9488,7 +9488,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -9572,7 +9572,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9610,7 +9610,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -9653,7 +9653,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10407,7 +10407,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10445,7 +10445,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -10530,7 +10530,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10568,7 +10568,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -10611,7 +10611,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11365,7 +11365,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11403,7 +11403,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -11487,7 +11487,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11525,7 +11525,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -11568,7 +11568,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12322,7 +12322,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12360,7 +12360,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1213121792"/>
@@ -12445,7 +12445,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="en-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12483,7 +12483,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1759877744"/>
@@ -12526,7 +12526,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -17987,8 +17987,8 @@
   </sheetPr>
   <dimension ref="A1:DJ176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18:K18"/>
     </sheetView>
   </sheetViews>
@@ -18034,32 +18034,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -18075,12 +18075,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="154"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -18088,12 +18088,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -18101,12 +18101,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="154"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -18114,12 +18114,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="156"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -18127,12 +18127,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="156"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -18180,112 +18180,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="159" t="s">
+      <c r="C13" s="163"/>
+      <c r="D13" s="165" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="165"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="165"/>
+      <c r="K13" s="165"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="159" t="s">
+      <c r="C14" s="163"/>
+      <c r="D14" s="165" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="165"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="165"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="159" t="s">
+      <c r="C15" s="163"/>
+      <c r="D15" s="165" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="159" t="str">
+      <c r="C16" s="163"/>
+      <c r="D16" s="165" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="157"/>
-      <c r="D17" s="159">
+      <c r="C17" s="163"/>
+      <c r="D17" s="165">
         <v>0.5</v>
       </c>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="157"/>
-      <c r="D18" s="158">
+      <c r="C18" s="163"/>
+      <c r="D18" s="164">
         <v>45365</v>
       </c>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -18473,16 +18473,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -20081,25 +20081,25 @@
         <v>-17.127219714134611</v>
       </c>
       <c r="AZ68" s="71">
-        <v>-7.0896214729580294</v>
+        <v>-7.0896214729580223</v>
       </c>
       <c r="BA68" s="71">
-        <v>9.046558991994516</v>
+        <v>9.0465589919945231</v>
       </c>
       <c r="BB68" s="71">
-        <v>26.06635477055708</v>
+        <v>26.066354770557087</v>
       </c>
       <c r="BC68" s="71">
-        <v>43.969765862729538</v>
+        <v>43.969765862729545</v>
       </c>
       <c r="BD68" s="71">
         <v>62.756792268512129</v>
       </c>
       <c r="BE68" s="71">
-        <v>82.42743398790472</v>
+        <v>82.427433987904735</v>
       </c>
       <c r="BF68" s="71">
-        <v>102.98169102090735</v>
+        <v>102.98169102090736</v>
       </c>
       <c r="BG68" s="71">
         <v>124.41956336751997</v>
@@ -20114,7 +20114,7 @@
         <v>194.03487228901781</v>
       </c>
       <c r="BK68" s="71">
-        <v>219.00720589007051</v>
+        <v>219.00720589007054</v>
       </c>
       <c r="BL68" s="71">
         <v>244.86315480473326</v>
@@ -21130,7 +21130,7 @@
       <c r="G119" s="11"/>
       <c r="H119" s="11"/>
       <c r="I119" s="80">
-        <v>43.993431730052762</v>
+        <v>43.99343173005277</v>
       </c>
       <c r="J119" s="80">
         <v>5.1464118389156249E-4</v>
@@ -22310,6 +22310,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -22326,10 +22330,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="23" priority="5" stopIfTrue="1" operator="between">
@@ -22415,32 +22415,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -22456,12 +22456,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="154"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -22469,12 +22469,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -22482,12 +22482,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="154"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -22495,12 +22495,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="156"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -22508,12 +22508,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="156"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -22561,117 +22561,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="159" t="str">
+      <c r="C13" s="163"/>
+      <c r="D13" s="165" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="165"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="165"/>
+      <c r="K13" s="165"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="159" t="str">
+      <c r="C14" s="163"/>
+      <c r="D14" s="165" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="165"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="165"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="159" t="str">
+      <c r="C15" s="163"/>
+      <c r="D15" s="165" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="159" t="str">
+      <c r="C16" s="163"/>
+      <c r="D16" s="165" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="157"/>
-      <c r="D17" s="159">
+      <c r="C17" s="163"/>
+      <c r="D17" s="165">
         <f>Gap30deg!D17</f>
         <v>0.5</v>
       </c>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="157"/>
-      <c r="D18" s="158">
+      <c r="C18" s="163"/>
+      <c r="D18" s="164">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -22859,16 +22859,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -26697,13 +26697,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -26717,6 +26710,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="20" priority="3" stopIfTrue="1" operator="between">
@@ -26802,32 +26802,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -26843,12 +26843,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="154"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -26856,12 +26856,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -26869,12 +26869,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="154"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -26882,12 +26882,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="156"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -26895,12 +26895,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="156"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -26948,117 +26948,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="159" t="str">
+      <c r="C13" s="163"/>
+      <c r="D13" s="165" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="165"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="165"/>
+      <c r="K13" s="165"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="159" t="str">
+      <c r="C14" s="163"/>
+      <c r="D14" s="165" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="165"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="165"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="159" t="str">
+      <c r="C15" s="163"/>
+      <c r="D15" s="165" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="159" t="str">
+      <c r="C16" s="163"/>
+      <c r="D16" s="165" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="157"/>
-      <c r="D17" s="159">
+      <c r="C17" s="163"/>
+      <c r="D17" s="165">
         <f>Gap30deg!D17</f>
         <v>0.5</v>
       </c>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="157"/>
-      <c r="D18" s="158">
+      <c r="C18" s="163"/>
+      <c r="D18" s="164">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -27246,16 +27246,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -31084,13 +31084,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -31104,6 +31097,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="between">
@@ -31189,32 +31189,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="160" t="s">
+      <c r="A3" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="161"/>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
-      <c r="F3" s="161"/>
-      <c r="G3" s="161"/>
-      <c r="H3" s="161"/>
-      <c r="I3" s="161"/>
-      <c r="J3" s="161"/>
-      <c r="K3" s="161"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="158"/>
+      <c r="H3" s="158"/>
+      <c r="I3" s="158"/>
+      <c r="J3" s="158"/>
+      <c r="K3" s="158"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="159"/>
+      <c r="E4" s="159"/>
+      <c r="F4" s="159"/>
+      <c r="G4" s="159"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -31230,12 +31230,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="154"/>
-      <c r="C5" s="155"/>
-      <c r="D5" s="155"/>
-      <c r="E5" s="155"/>
-      <c r="F5" s="155"/>
-      <c r="G5" s="156"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="161"/>
+      <c r="D5" s="161"/>
+      <c r="E5" s="161"/>
+      <c r="F5" s="161"/>
+      <c r="G5" s="162"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -31243,12 +31243,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="154"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="155"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="155"/>
-      <c r="G6" s="156"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="162"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -31256,12 +31256,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="154"/>
-      <c r="C7" s="155"/>
-      <c r="D7" s="155"/>
-      <c r="E7" s="155"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="156"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
+      <c r="D7" s="161"/>
+      <c r="E7" s="161"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="162"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -31269,12 +31269,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="154"/>
-      <c r="C8" s="155"/>
-      <c r="D8" s="155"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="155"/>
-      <c r="G8" s="156"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="161"/>
+      <c r="D8" s="161"/>
+      <c r="E8" s="161"/>
+      <c r="F8" s="161"/>
+      <c r="G8" s="162"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -31282,12 +31282,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="154"/>
-      <c r="C9" s="155"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="155"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="156"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="161"/>
+      <c r="D9" s="161"/>
+      <c r="E9" s="161"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="162"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -31335,117 +31335,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="163" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="157"/>
-      <c r="D13" s="159" t="str">
+      <c r="C13" s="163"/>
+      <c r="D13" s="165" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="159"/>
-      <c r="F13" s="159"/>
-      <c r="G13" s="159"/>
-      <c r="H13" s="159"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
-      <c r="K13" s="159"/>
+      <c r="E13" s="165"/>
+      <c r="F13" s="165"/>
+      <c r="G13" s="165"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="165"/>
+      <c r="K13" s="165"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="163" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="159" t="str">
+      <c r="C14" s="163"/>
+      <c r="D14" s="165" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="159"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="159"/>
-      <c r="H14" s="159"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
-      <c r="K14" s="159"/>
+      <c r="E14" s="165"/>
+      <c r="F14" s="165"/>
+      <c r="G14" s="165"/>
+      <c r="H14" s="165"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="165"/>
+      <c r="K14" s="165"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="157" t="s">
+      <c r="B15" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="159" t="str">
+      <c r="C15" s="163"/>
+      <c r="D15" s="165" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="157" t="s">
+      <c r="B16" s="163" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="157"/>
-      <c r="D16" s="159" t="str">
+      <c r="C16" s="163"/>
+      <c r="D16" s="165" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="163" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="157"/>
-      <c r="D17" s="159">
+      <c r="C17" s="163"/>
+      <c r="D17" s="165">
         <f>Gap30deg!D17</f>
         <v>0.5</v>
       </c>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="157" t="s">
+      <c r="B18" s="163" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="157"/>
-      <c r="D18" s="158">
+      <c r="C18" s="163"/>
+      <c r="D18" s="164">
         <f>Gap30deg!D18</f>
         <v>45365</v>
       </c>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
+      <c r="E18" s="164"/>
+      <c r="F18" s="164"/>
+      <c r="G18" s="164"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="164"/>
+      <c r="J18" s="164"/>
+      <c r="K18" s="164"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -31633,16 +31633,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="163"/>
-      <c r="C28" s="164"/>
-      <c r="D28" s="164"/>
-      <c r="E28" s="164"/>
-      <c r="F28" s="164"/>
-      <c r="G28" s="164"/>
-      <c r="H28" s="164"/>
-      <c r="I28" s="164"/>
-      <c r="J28" s="164"/>
-      <c r="K28" s="165"/>
+      <c r="B28" s="154"/>
+      <c r="C28" s="155"/>
+      <c r="D28" s="155"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="155"/>
+      <c r="I28" s="155"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -35471,13 +35471,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -35491,6 +35484,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="between">
@@ -35526,9 +35526,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC92106B-D6AD-4F84-9466-7FC5961EFD60}">
   <dimension ref="B2:Q106"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="26" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -38894,23 +38894,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -39163,10 +39146,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39189,20 +39200,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>